<commit_message>
latest in scrum board
</commit_message>
<xml_diff>
--- a/scrum_board.xlsx
+++ b/scrum_board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A393350\Desktop\Kaggle\AceaSmartWaterAnalytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250EFB12-77CC-4C06-AFAB-AE8EDD90E5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B73256F-6AFE-49F2-B6A9-78F5067D1EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6B62BD1B-31D1-4B4A-B60E-AE30911C9554}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>To-Do</t>
   </si>
@@ -45,15 +45,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Recurrent Neural Networks</t>
-  </si>
-  <si>
-    <t>LSTM for univariate time series</t>
-  </si>
-  <si>
-    <t>Autoregressive Convolutional Recurrent Neural Netowrk</t>
-  </si>
-  <si>
     <t>Univariate time series forecast of Aquifer Patrignano</t>
   </si>
   <si>
@@ -64,6 +55,21 @@
   </si>
   <si>
     <t>Improve ARIMA existing model</t>
+  </si>
+  <si>
+    <t>Products demand (https://www.datacamp.com/courses/forecasting-product-demand-in-r)</t>
+  </si>
+  <si>
+    <t>Dada studying forecasting methods (https://www.datacamp.com/tutorial/tutorial-time-series-forecasting?irclickid=Qu-WEL35QxyIRzmX30wL5WzCUkD2--zut0y1wg0&amp;irgwc=1&amp;utm_medium=affiliate&amp;utm_source=impact&amp;utm_campaign=1310690#what-is-time-series-forecasting-)</t>
+  </si>
+  <si>
+    <t>Classical / Statistical Models — Moving Averages, Exponential Smoothing, ARIMA, SARIMA, TBATS</t>
+  </si>
+  <si>
+    <t>Machine Learning — Linear Regression, XGBoost, Random Forest, or any ML model with reduction methods</t>
+  </si>
+  <si>
+    <t>Deep Learning — RNN, LSTM, Autoregressive CNN for univariate time series / multivariate</t>
   </si>
 </sst>
 </file>
@@ -447,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D83F88-49C4-4FAD-9EB4-B9235DFA2BEC}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.54296875" customWidth="1"/>
     <col min="2" max="2" width="45.81640625" customWidth="1"/>
     <col min="3" max="3" width="52.90625" customWidth="1"/>
   </cols>
@@ -472,31 +478,45 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2 new notebooks and updates in scrum board
</commit_message>
<xml_diff>
--- a/scrum_board.xlsx
+++ b/scrum_board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A393350\Desktop\Kaggle\AceaSmartWaterAnalytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B73256F-6AFE-49F2-B6A9-78F5067D1EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E14814-32B4-4FAD-AF72-EDE14CF699F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6B62BD1B-31D1-4B4A-B60E-AE30911C9554}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>start ARIMA</t>
   </si>
   <si>
-    <t>Improve ARIMA existing model</t>
-  </si>
-  <si>
     <t>Products demand (https://www.datacamp.com/courses/forecasting-product-demand-in-r)</t>
   </si>
   <si>
@@ -70,6 +67,10 @@
   </si>
   <si>
     <t>Deep Learning — RNN, LSTM, Autoregressive CNN for univariate time series / multivariate</t>
+  </si>
+  <si>
+    <t>Create prediction and interpretation of results for Aquifers and Water Spring in 2 separate notebooks as:
+- baseline model (such as e.g. ARIMA) on univariate analysis and get conclusions</t>
   </si>
 </sst>
 </file>
@@ -131,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -139,6 +140,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,21 +484,21 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -501,7 +506,7 @@
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -509,11 +514,8 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>

</xml_diff>

<commit_message>
update in the scrum board
</commit_message>
<xml_diff>
--- a/scrum_board.xlsx
+++ b/scrum_board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A393350\Desktop\Kaggle\AceaSmartWaterAnalytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E14814-32B4-4FAD-AF72-EDE14CF699F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA7CDF8-520D-42C4-BDC3-B729AF676AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6B62BD1B-31D1-4B4A-B60E-AE30911C9554}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>To-Do</t>
   </si>
@@ -71,6 +71,12 @@
   <si>
     <t>Create prediction and interpretation of results for Aquifers and Water Spring in 2 separate notebooks as:
 - baseline model (such as e.g. ARIMA) on univariate analysis and get conclusions</t>
+  </si>
+  <si>
+    <t>CatBoost Regressor</t>
+  </si>
+  <si>
+    <t>https://openai.com/dall-e-2/</t>
   </si>
 </sst>
 </file>
@@ -461,7 +467,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -517,8 +523,15 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>